<commit_message>
2024 ready to go
</commit_message>
<xml_diff>
--- a/SB_Squares_2024.xlsx
+++ b/SB_Squares_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmari\Documents\Repos\sb-squares-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7B42E1-8A57-4132-A9EC-20DF3209F098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EF7F48-407C-4F31-B09C-8E787329A997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SB_Squares_2024" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="21">
   <si>
     <t>Participants</t>
+  </si>
+  <si>
+    <t>Favero, Gian</t>
+  </si>
+  <si>
+    <t>Ogley, Andrew</t>
+  </si>
+  <si>
+    <t>Iannetta, Adrian</t>
+  </si>
+  <si>
+    <t>Ammoscato, Matt</t>
+  </si>
+  <si>
+    <t>Amlin, Brayden</t>
+  </si>
+  <si>
+    <t>Byrne, Thomas</t>
+  </si>
+  <si>
+    <t>Caro, Steven</t>
+  </si>
+  <si>
+    <t>Hill, Stevie</t>
+  </si>
+  <si>
+    <t>Scholl, Noah</t>
+  </si>
+  <si>
+    <t>McVinnie, Robert</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>GF</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>TB</t>
   </si>
 </sst>
 </file>
@@ -179,13 +239,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Amasis MT Pro Black"/>
@@ -196,6 +249,13 @@
       <color theme="1"/>
       <name val="Bodoni MT"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="37">
@@ -723,15 +783,6 @@
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -744,7 +795,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -775,13 +826,22 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1896,19 +1956,19 @@
   </sheetPr>
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="41" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:O12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="13" width="9" customWidth="1"/>
-    <col min="15" max="15" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="121.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="121.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23"/>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1926,9 +1986,9 @@
       <c r="O1" s="24"/>
       <c r="P1" s="25"/>
     </row>
-    <row r="2" spans="1:16" ht="112.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="12"/>
+    <row r="2" spans="1:16" ht="112.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
@@ -1940,269 +2000,489 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
       <c r="M2" s="27"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="19"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
+    <row r="3" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
       <c r="B3" s="28"/>
-      <c r="C3" s="1">
+      <c r="C3" s="20">
         <v>2024</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="21">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="21">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="21">
         <v>2</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="21">
         <v>3</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="21">
         <v>4</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="21">
         <v>5</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="21">
         <v>6</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="21">
         <v>7</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="21">
         <v>8</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="10">
         <v>9</v>
       </c>
-      <c r="N3" s="20"/>
-      <c r="O3" s="8" t="s">
+      <c r="N3" s="17"/>
+      <c r="O3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="19"/>
+      <c r="P3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
+    <row r="4" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
       <c r="B4" s="28"/>
-      <c r="C4" s="2">
+      <c r="C4" s="21">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="19"/>
+      <c r="D4" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="17"/>
+      <c r="O4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
+    <row r="5" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
       <c r="B5" s="28"/>
-      <c r="C5" s="2">
+      <c r="C5" s="21">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="19"/>
+      <c r="D5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="17"/>
+      <c r="O5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
+    <row r="6" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
       <c r="B6" s="28"/>
-      <c r="C6" s="2">
+      <c r="C6" s="21">
         <v>2</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="19"/>
+      <c r="D6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="17"/>
+      <c r="O6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="16"/>
     </row>
-    <row r="7" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
+    <row r="7" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
       <c r="B7" s="28"/>
-      <c r="C7" s="2">
+      <c r="C7" s="21">
         <v>3</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="19"/>
+      <c r="D7" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="17"/>
+      <c r="O7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="16"/>
     </row>
-    <row r="8" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
+    <row r="8" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
       <c r="B8" s="28"/>
-      <c r="C8" s="2">
+      <c r="C8" s="21">
         <v>4</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="19"/>
+      <c r="D8" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="17"/>
+      <c r="O8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="16"/>
     </row>
-    <row r="9" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
+    <row r="9" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
       <c r="B9" s="28"/>
-      <c r="C9" s="2">
+      <c r="C9" s="21">
         <v>5</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="19"/>
+      <c r="D9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="17"/>
+      <c r="O9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="16"/>
     </row>
-    <row r="10" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
+    <row r="10" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
       <c r="B10" s="28"/>
-      <c r="C10" s="2">
+      <c r="C10" s="21">
         <v>6</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="19"/>
+      <c r="D10" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="17"/>
+      <c r="O10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="16"/>
     </row>
-    <row r="11" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
+    <row r="11" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
       <c r="B11" s="28"/>
-      <c r="C11" s="2">
+      <c r="C11" s="21">
         <v>7</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="19"/>
+      <c r="D11" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="17"/>
+      <c r="O11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="16"/>
     </row>
-    <row r="12" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
+    <row r="12" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
       <c r="B12" s="28"/>
-      <c r="C12" s="2">
+      <c r="C12" s="21">
         <v>8</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="19"/>
+      <c r="D12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="17"/>
+      <c r="O12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="16"/>
     </row>
-    <row r="13" spans="1:16" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="22"/>
+    <row r="13" spans="1:16" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
       <c r="B13" s="29"/>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>9</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="19"/>
+      <c r="D13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" s="17"/>
+      <c r="O13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P13" s="16"/>
     </row>
-    <row r="14" spans="1:16" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="18"/>
+    <row r="14" spans="1:16" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2211,7 +2491,7 @@
     <mergeCell ref="B3:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="61" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="63" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>